<commit_message>
Adding title name at top of nav. Prepping for css grid
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trancjo/Documents/JordanTranchina.github.io/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A80517-4599-3947-ADAD-4EA427C403EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA7D5250-F274-0242-9AB8-C1DEE7172B0F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33400" windowHeight="19440" activeTab="1" xr2:uid="{1028C8D6-223D-9241-9794-8257F6E37852}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19440" activeTab="2" xr2:uid="{1028C8D6-223D-9241-9794-8257F6E37852}"/>
   </bookViews>
   <sheets>
     <sheet name="Breakpoint Calculations" sheetId="1" r:id="rId1"/>
     <sheet name="Skills" sheetId="2" r:id="rId2"/>
+    <sheet name="Grid_Mobile" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
   <si>
     <t>Total Page Size</t>
   </si>
@@ -125,6 +126,33 @@
   </si>
   <si>
     <t>%</t>
+  </si>
+  <si>
+    <t>Column 1</t>
+  </si>
+  <si>
+    <t>Column 2</t>
+  </si>
+  <si>
+    <t>Column 3</t>
+  </si>
+  <si>
+    <t>Column 4</t>
+  </si>
+  <si>
+    <t>Margin</t>
+  </si>
+  <si>
+    <t>Gutter</t>
+  </si>
+  <si>
+    <t>auto</t>
+  </si>
+  <si>
+    <t>Dimensions</t>
+  </si>
+  <si>
+    <t>16px</t>
   </si>
 </sst>
 </file>
@@ -645,7 +673,7 @@
   <dimension ref="B1:K12"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="200" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -994,7 +1022,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C1B58C4-3778-3C49-B299-BFF8DA0593A2}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
@@ -1296,4 +1324,83 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76938D92-0B74-6144-B0F8-6EBE2ACD9554}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Changed nav bar to horizontal in a grid
</commit_message>
<xml_diff>
--- a/Calculations.xlsx
+++ b/Calculations.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trancjo/Documents/JordanTranchina.github.io/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA7D5250-F274-0242-9AB8-C1DEE7172B0F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05AD24D2-E80E-E64E-AB4C-1F1FE1E432FA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19440" activeTab="2" xr2:uid="{1028C8D6-223D-9241-9794-8257F6E37852}"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="33600" windowHeight="19440" activeTab="3" xr2:uid="{1028C8D6-223D-9241-9794-8257F6E37852}"/>
   </bookViews>
   <sheets>
     <sheet name="Breakpoint Calculations" sheetId="1" r:id="rId1"/>
     <sheet name="Skills" sheetId="2" r:id="rId2"/>
     <sheet name="Grid_Mobile" sheetId="3" r:id="rId3"/>
+    <sheet name="Grid_TabletPortrait" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="58">
   <si>
     <t>Total Page Size</t>
   </si>
@@ -140,6 +141,12 @@
     <t>Column 4</t>
   </si>
   <si>
+    <t>Column 5</t>
+  </si>
+  <si>
+    <t>Column 6</t>
+  </si>
+  <si>
     <t>Margin</t>
   </si>
   <si>
@@ -153,6 +160,48 @@
   </si>
   <si>
     <t>16px</t>
+  </si>
+  <si>
+    <t>Nav</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>logo (left aligned)</t>
+  </si>
+  <si>
+    <t>about (centered)</t>
+  </si>
+  <si>
+    <t>work (centered)</t>
+  </si>
+  <si>
+    <t>Column 7</t>
+  </si>
+  <si>
+    <t>Column 8</t>
+  </si>
+  <si>
+    <t>24px</t>
+  </si>
+  <si>
+    <t>Education (centered)</t>
+  </si>
+  <si>
+    <t>Work (centered)</t>
+  </si>
+  <si>
+    <t>About (centered)</t>
+  </si>
+  <si>
+    <t>Logo (left aligned)</t>
+  </si>
+  <si>
+    <t>Contact (centered)</t>
+  </si>
+  <si>
+    <t>Jordan Tranchina (right-aligned)</t>
   </si>
 </sst>
 </file>
@@ -339,7 +388,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -355,6 +404,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1328,76 +1380,247 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76938D92-0B74-6144-B0F8-6EBE2ACD9554}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="10" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s">
         <v>33</v>
       </c>
       <c r="D1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E1" t="s">
         <v>34</v>
       </c>
       <c r="F1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G1" t="s">
         <v>35</v>
       </c>
       <c r="H1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I1" t="s">
         <v>36</v>
       </c>
       <c r="J1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC6C024C-7902-F44D-BED5-CCAA6F00823E}">
+  <dimension ref="A1:R3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="18" width="15.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
         <v>40</v>
       </c>
+      <c r="E1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>50</v>
+      </c>
+      <c r="R1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
       <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
         <v>41</v>
       </c>
-      <c r="C2" t="s">
-        <v>39</v>
-      </c>
       <c r="D2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" t="s">
         <v>41</v>
       </c>
-      <c r="E2" t="s">
-        <v>39</v>
-      </c>
       <c r="F2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" t="s">
         <v>41</v>
       </c>
-      <c r="G2" t="s">
-        <v>39</v>
-      </c>
       <c r="H2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" t="s">
         <v>41</v>
       </c>
-      <c r="I2" t="s">
-        <v>39</v>
-      </c>
       <c r="J2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2" t="s">
         <v>41</v>
+      </c>
+      <c r="L2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M2" t="s">
+        <v>41</v>
+      </c>
+      <c r="N2" t="s">
+        <v>43</v>
+      </c>
+      <c r="O2" t="s">
+        <v>41</v>
+      </c>
+      <c r="P2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>41</v>
+      </c>
+      <c r="R2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I3" t="s">
+        <v>52</v>
+      </c>
+      <c r="K3" t="s">
+        <v>56</v>
+      </c>
+      <c r="M3" t="s">
+        <v>45</v>
+      </c>
+      <c r="O3" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q3" s="15" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>